<commit_message>
done messages function & grade function
</commit_message>
<xml_diff>
--- a/student/upload/uploads/37732-new-microsoft-excel-worksheet.xlsx
+++ b/student/upload/uploads/37732-new-microsoft-excel-worksheet.xlsx
@@ -16,10 +16,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -369,20 +365,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>